<commit_message>
HumanHand results files are now pickable.
</commit_message>
<xml_diff>
--- a/Setup/LoadDimensions_humanhand.xlsx
+++ b/Setup/LoadDimensions_humanhand.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>width</t>
   </si>
@@ -36,6 +36,12 @@
   </si>
   <si>
     <t>length</t>
+  </si>
+  <si>
+    <t>12.9</t>
+  </si>
+  <si>
+    <t>0.9</t>
   </si>
 </sst>
 </file>
@@ -389,11 +395,11 @@
       <c r="A2">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>12.9</v>
-      </c>
-      <c r="C2">
-        <v>0.9</v>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
       <c r="D2">
         <v>3</v>

</xml_diff>